<commit_message>
Amend corrected label annotations
</commit_message>
<xml_diff>
--- a/example_data/EMA/label_corrected/abilify-epar-product-information_en.xlsx
+++ b/example_data/EMA/label_corrected/abilify-epar-product-information_en.xlsx
@@ -13021,7 +13021,7 @@
       </c>
       <c r="H332" t="inlineStr">
         <is>
-          <t>populations - adult || populations - geriatric</t>
+          <t>populations - geriatric || populations - adult</t>
         </is>
       </c>
       <c r="I332" t="inlineStr"/>
@@ -19381,7 +19381,7 @@
       </c>
       <c r="H501" t="inlineStr">
         <is>
-          <t>populations - adult || populations - geriatric</t>
+          <t>populations - geriatric || populations - adult</t>
         </is>
       </c>
       <c r="I501" t="inlineStr"/>
@@ -24998,7 +24998,7 @@
       </c>
       <c r="H656" t="inlineStr">
         <is>
-          <t>populations - adult || populations - geriatric</t>
+          <t>populations - geriatric || populations - adult</t>
         </is>
       </c>
       <c r="I656" t="inlineStr"/>

</xml_diff>